<commit_message>
correct bacillus graph with other demarcations added
</commit_message>
<xml_diff>
--- a/results/Lingparallelizedes2.xlsx
+++ b/results/Lingparallelizedes2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3220" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="include demarcation" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="33">
   <si>
     <t>Num of Cores:</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>$Hillclimbing_i/Hillclimbing_1$</t>
+  </si>
+  <si>
+    <t>amended for error…</t>
   </si>
 </sst>
 </file>
@@ -599,25 +602,25 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.658329398280063</c:v>
+                  <c:v>0.6663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.555486765634981</c:v>
+                  <c:v>0.5622</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.426096141812873</c:v>
+                  <c:v>0.4313</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36749285840031</c:v>
+                  <c:v>0.372</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.360206956942421</c:v>
+                  <c:v>0.3669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.313428538328259</c:v>
+                  <c:v>0.3172</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.312803326833804</c:v>
+                  <c:v>0.3086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,25 +679,25 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.078996420809271</c:v>
+                  <c:v>1.0789</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.943316279387159</c:v>
+                  <c:v>0.9432</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.825861326787055</c:v>
+                  <c:v>0.8258</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.707817665990425</c:v>
+                  <c:v>0.7078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.610821040756383</c:v>
+                  <c:v>0.6246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67001348090576</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.629955678590265</c:v>
+                  <c:v>0.6053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -753,25 +756,25 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.484973848581674</c:v>
+                  <c:v>0.487</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.327229580405207</c:v>
+                  <c:v>0.3286</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.243460786462076</c:v>
+                  <c:v>0.2445</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.253375393035688</c:v>
+                  <c:v>0.2544</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.215226558295116</c:v>
+                  <c:v>0.2124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.151675168638003</c:v>
+                  <c:v>0.1523</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.124066084199398</c:v>
+                  <c:v>0.1326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -830,25 +833,25 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.635981862178569</c:v>
+                  <c:v>0.6441</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.534983811464359</c:v>
+                  <c:v>0.5418</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.404840744002964</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.349294033750964</c:v>
+                  <c:v>0.3538</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.346882306873242</c:v>
+                  <c:v>0.353</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.294432186143135</c:v>
+                  <c:v>0.2982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.295975408777107</c:v>
+                  <c:v>0.2926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -863,11 +866,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2062185368"/>
-        <c:axId val="2062192280"/>
+        <c:axId val="2099131272"/>
+        <c:axId val="2099136808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2062185368"/>
+        <c:axId val="2099131272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -898,12 +901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062192280"/>
+        <c:crossAx val="2099136808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2062192280"/>
+        <c:axId val="2099136808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062185368"/>
+        <c:crossAx val="2099131272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1046,11 +1049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2062269144"/>
-        <c:axId val="2062272152"/>
+        <c:axId val="2099170056"/>
+        <c:axId val="2099173000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2062269144"/>
+        <c:axId val="2099170056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062272152"/>
+        <c:crossAx val="2099173000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1067,7 +1070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062272152"/>
+        <c:axId val="2099173000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1081,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062269144"/>
+        <c:crossAx val="2099170056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1227,11 +1230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2062307720"/>
-        <c:axId val="2062310696"/>
+        <c:axId val="2099204760"/>
+        <c:axId val="2099207736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2062307720"/>
+        <c:axId val="2099204760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062310696"/>
+        <c:crossAx val="2099207736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1248,7 +1251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062310696"/>
+        <c:axId val="2099207736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062307720"/>
+        <c:crossAx val="2099204760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1284,15 +1287,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1704,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2283,37 +2286,29 @@
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6">
-        <f>B6/B6</f>
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C13" s="6">
-        <f>C6/B6</f>
-        <v>0.65832939828006309</v>
-      </c>
-      <c r="D13" s="6">
-        <f>D6/B6</f>
-        <v>0.55548676563498145</v>
-      </c>
-      <c r="E13" s="6">
-        <f>E6/B6</f>
-        <v>0.42609614181287253</v>
-      </c>
-      <c r="F13" s="6">
-        <f>F6/B6</f>
-        <v>0.36749285840031048</v>
-      </c>
-      <c r="G13" s="6">
-        <f>G6/B6</f>
-        <v>0.36020695694242066</v>
-      </c>
-      <c r="H13" s="6">
-        <f>H6/B6</f>
-        <v>0.31342853832825934</v>
-      </c>
-      <c r="I13" s="6">
-        <f>I6/B6</f>
-        <v>0.31280332683380407</v>
+      <c r="C13" s="7">
+        <v>0.6663</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.56220000000000003</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.43130000000000002</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.372</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0.3669</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0.31719999999999998</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0.30859999999999999</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -2325,37 +2320,29 @@
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6">
-        <f>B3/B3</f>
+      <c r="B14" s="7">
         <v>1</v>
       </c>
-      <c r="C14" s="6">
-        <f>C3/B3</f>
-        <v>1.0789964208092708</v>
-      </c>
-      <c r="D14" s="6">
-        <f>D3/B3</f>
-        <v>0.94331627938715945</v>
-      </c>
-      <c r="E14" s="6">
-        <f>E3/B3</f>
-        <v>0.82586132678705493</v>
-      </c>
-      <c r="F14" s="6">
-        <f>F3/B3</f>
-        <v>0.70781766599042517</v>
-      </c>
-      <c r="G14" s="6">
-        <f>G3/B3</f>
-        <v>0.61082104075638344</v>
-      </c>
-      <c r="H14" s="6">
-        <f>H3/B3</f>
-        <v>0.67001348090576007</v>
-      </c>
-      <c r="I14" s="6">
-        <f>I3/B3</f>
-        <v>0.6299556785902648</v>
+      <c r="C14" s="7">
+        <v>1.0789</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.82579999999999998</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.70779999999999998</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.62460000000000004</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.67</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.60529999999999995</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -2367,37 +2354,29 @@
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="6">
-        <f>B4/B4</f>
+      <c r="B15" s="7">
         <v>1</v>
       </c>
-      <c r="C15" s="6">
-        <f>C4/B4</f>
-        <v>0.48497384858167408</v>
-      </c>
-      <c r="D15" s="6">
-        <f>D4/B4</f>
-        <v>0.32722958040520683</v>
-      </c>
-      <c r="E15" s="6">
-        <f>E4/B4</f>
-        <v>0.24346078646207578</v>
-      </c>
-      <c r="F15" s="6">
-        <f>F4/B4</f>
-        <v>0.2533753930356879</v>
-      </c>
-      <c r="G15" s="6">
-        <f>G4/B4</f>
-        <v>0.21522655829511594</v>
-      </c>
-      <c r="H15" s="6">
-        <f>H4/B4</f>
-        <v>0.1516751686380029</v>
-      </c>
-      <c r="I15" s="6">
-        <f>I4/B4</f>
-        <v>0.12406608419939782</v>
+      <c r="C15" s="7">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.3286</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.2445</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.1326</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -2409,37 +2388,29 @@
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="6">
-        <f>B5/B5</f>
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16" s="6">
-        <f>C5/B5</f>
-        <v>0.63598186217856889</v>
-      </c>
-      <c r="D16" s="6">
-        <f>D5/B5</f>
-        <v>0.53498381146435947</v>
-      </c>
-      <c r="E16" s="6">
-        <f>E5/B5</f>
-        <v>0.40484074400296355</v>
-      </c>
-      <c r="F16" s="6">
-        <f>F5/B5</f>
-        <v>0.34929403375096446</v>
-      </c>
-      <c r="G16" s="6">
-        <f>G5/B5</f>
-        <v>0.34688230687324245</v>
-      </c>
-      <c r="H16" s="6">
-        <f>H5/B5</f>
-        <v>0.2944321861431351</v>
-      </c>
-      <c r="I16" s="6">
-        <f>I5/B5</f>
-        <v>0.2959754087771066</v>
+      <c r="C16" s="7">
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.54179999999999995</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.41</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.3538</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.29820000000000002</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.29260000000000003</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -2448,6 +2419,9 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:17">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>

</xml_diff>